<commit_message>
ocr updates, streamlit app updates
</commit_message>
<xml_diff>
--- a/fig_pages_viewed.xlsx
+++ b/fig_pages_viewed.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G139"/>
+  <dimension ref="A1:G144"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4196,6 +4196,141 @@
         <v>0</v>
       </c>
     </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Allard-Poesi &amp; Hollet-Haudebert_2021_HR_The Sound of Silence Measuring Suffering at Work.pdf</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>F2_P12_Allard-Poesi &amp; Hollet-Haudebert_2021_HR_The Sound of Silence Measuring Suffering at Work.png</t>
+        </is>
+      </c>
+      <c r="C140" t="n">
+        <v>2</v>
+      </c>
+      <c r="D140" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E140" t="n">
+        <v>13</v>
+      </c>
+      <c r="F140" t="n">
+        <v>0</v>
+      </c>
+      <c r="G140" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Allard-Poesi &amp; Hollet-Haudebert_2021_HR_The Sound of Silence Measuring Suffering at Work.pdf</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>F2_P11_Allard-Poesi &amp; Hollet-Haudebert_2021_HR_The Sound of Silence Measuring Suffering at Work.png</t>
+        </is>
+      </c>
+      <c r="C141" t="n">
+        <v>2</v>
+      </c>
+      <c r="D141" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E141" t="n">
+        <v>12</v>
+      </c>
+      <c r="F141" t="n">
+        <v>0</v>
+      </c>
+      <c r="G141" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>Allard-Poesi &amp; Hollet-Haudebert_2021_HR_The Sound of Silence Measuring Suffering at Work.pdf</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>F3_P12_Allard-Poesi &amp; Hollet-Haudebert_2021_HR_The Sound of Silence Measuring Suffering at Work.png</t>
+        </is>
+      </c>
+      <c r="C142" t="n">
+        <v>3</v>
+      </c>
+      <c r="D142" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E142" t="n">
+        <v>13</v>
+      </c>
+      <c r="F142" t="n">
+        <v>0</v>
+      </c>
+      <c r="G142" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Anthony_2021_ASQ_When Knowledge Work and Analytical Technology Collide.pdf</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>F1_P6_Anthony_2021_ASQ_When Knowledge Work and Analytical Technology Collide.png</t>
+        </is>
+      </c>
+      <c r="C143" t="n">
+        <v>1</v>
+      </c>
+      <c r="D143" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E143" t="n">
+        <v>7</v>
+      </c>
+      <c r="F143" t="n">
+        <v>0</v>
+      </c>
+      <c r="G143" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Anthony_2021_ASQ_When Knowledge Work and Analytical Technology Collide.pdf</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>F2_P6_Anthony_2021_ASQ_When Knowledge Work and Analytical Technology Collide.png</t>
+        </is>
+      </c>
+      <c r="C144" t="n">
+        <v>2</v>
+      </c>
+      <c r="D144" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E144" t="n">
+        <v>7</v>
+      </c>
+      <c r="F144" t="n">
+        <v>0</v>
+      </c>
+      <c r="G144" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
that one datatype error - bane of my existence - handled
</commit_message>
<xml_diff>
--- a/fig_pages_viewed.xlsx
+++ b/fig_pages_viewed.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G144"/>
+  <dimension ref="A1:G148"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4331,6 +4331,114 @@
         <v>0</v>
       </c>
     </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Creary &amp; Locke_2022_OrgSci_Breaking hte Cycle of Overwork and Recuperation.pdf</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>F1_P13_Creary &amp; Locke_2022_OrgSci_Breaking hte Cycle of Overwork and Recuperation.png</t>
+        </is>
+      </c>
+      <c r="C145" t="n">
+        <v>1</v>
+      </c>
+      <c r="D145" t="n">
+        <v>2022</v>
+      </c>
+      <c r="E145" t="n">
+        <v>14</v>
+      </c>
+      <c r="F145" t="n">
+        <v>0</v>
+      </c>
+      <c r="G145" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Anthony_2021_ASQ_When Knowledge Work and Analytical Technology Collide.pdf</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>F2_P7_Anthony_2021_ASQ_When Knowledge Work and Analytical Technology Collide.png</t>
+        </is>
+      </c>
+      <c r="C146" t="n">
+        <v>2</v>
+      </c>
+      <c r="D146" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E146" t="n">
+        <v>8</v>
+      </c>
+      <c r="F146" t="n">
+        <v>0</v>
+      </c>
+      <c r="G146" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Aoki_2020_AMJ_The Roles of Material Artfifacts in Managing the Learning Performance Paradox.pdf</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>F1_P12_Aoki_2020_AMJ_The Roles of Material Artfifacts in Managing the Learning Performance Paradox.png</t>
+        </is>
+      </c>
+      <c r="C147" t="n">
+        <v>1</v>
+      </c>
+      <c r="D147" t="n">
+        <v>2020</v>
+      </c>
+      <c r="E147" t="n">
+        <v>13</v>
+      </c>
+      <c r="F147" t="n">
+        <v>0</v>
+      </c>
+      <c r="G147" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Anthony_2021_ASQ_When Knowledge Work and Analytical Technology Collide.pdf</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>F2_P21_Anthony_2021_ASQ_When Knowledge Work and Analytical Technology Collide.png</t>
+        </is>
+      </c>
+      <c r="C148" t="n">
+        <v>2</v>
+      </c>
+      <c r="D148" t="n">
+        <v>2021</v>
+      </c>
+      <c r="E148" t="n">
+        <v>22</v>
+      </c>
+      <c r="F148" t="n">
+        <v>0</v>
+      </c>
+      <c r="G148" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>